<commit_message>
Modify data, remove unused code
</commit_message>
<xml_diff>
--- a/src/res/customerDetails.xlsx
+++ b/src/res/customerDetails.xlsx
@@ -9,7 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -626,7 +626,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
+      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1264,8 +1264,8 @@
   </sheetPr>
   <dimension ref="E6:S44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>